<commit_message>
Stack calculations for 50 MeV is done and I had to run 30MeV again because of some missing kapton ad
</commit_message>
<xml_diff>
--- a/50MeV_stack_analysis/50MeV_Ti_Fe_Zr_Foils.xlsx
+++ b/50MeV_stack_analysis/50MeV_Ti_Fe_Zr_Foils.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d50fdffd1f97c7a6/Dokumenter/Master/Master-project-code/50MeV_stack_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="268" documentId="14_{7FE2433E-3551-A74B-8720-1D259C5F8435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{024696FD-4E81-8849-9E0A-D2F64D19AC32}"/>
+  <xr:revisionPtr revIDLastSave="285" documentId="14_{7FE2433E-3551-A74B-8720-1D259C5F8435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E358062F-7E5B-5E4D-AE81-C7ABE919A646}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zr" sheetId="1" r:id="rId1"/>
@@ -165,7 +165,7 @@
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -205,8 +205,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -223,6 +230,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -267,7 +280,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -368,6 +381,12 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -383,6 +402,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -687,8 +710,8 @@
   </sheetPr>
   <dimension ref="A1:AE1000"/>
   <sheetViews>
-    <sheetView zoomScale="200" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -815,7 +838,7 @@
         <f t="array" ref="M2">SQRT(AVERAGE(L2:L5^2))</f>
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="N2" s="19">
+      <c r="N2" s="47">
         <f>M2/(G2*I2)*1000*100</f>
         <v>16.177424202819875</v>
       </c>
@@ -1045,7 +1068,7 @@
         <f t="array" ref="M8">SQRT(AVERAGE(L8:L11^2))</f>
         <v>0.1</v>
       </c>
-      <c r="N8" s="19">
+      <c r="N8" s="47">
         <f>M8/(G8*I8)*1000*100</f>
         <v>16.009059494908893</v>
       </c>
@@ -1255,7 +1278,7 @@
         <f t="array" ref="M14">SQRT(AVERAGE(L14:L17^2))</f>
         <v>0.10199999999999999</v>
       </c>
-      <c r="N14" s="19">
+      <c r="N14" s="47">
         <f>M14/(G14*I14)*1000*100</f>
         <v>16.246176798893259</v>
       </c>
@@ -1465,7 +1488,7 @@
         <f t="array" ref="M20">SQRT(AVERAGE(L20:L23^2))</f>
         <v>0.10199999999999999</v>
       </c>
-      <c r="N20" s="19">
+      <c r="N20" s="47">
         <f>M20/(G20*I20)*1000*100</f>
         <v>16.22454164422361</v>
       </c>
@@ -1675,7 +1698,7 @@
         <f t="array" ref="M26">SQRT(AVERAGE(L26:L29^2))</f>
         <v>0.10299999999999999</v>
       </c>
-      <c r="N26" s="19">
+      <c r="N26" s="47">
         <f>M26/(G26*I26)*1000*100</f>
         <v>16.236779710109914</v>
       </c>
@@ -14800,8 +14823,8 @@
   </sheetPr>
   <dimension ref="A1:AE1000"/>
   <sheetViews>
-    <sheetView zoomScale="175" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -14928,7 +14951,7 @@
         <f t="array" ref="M2">SQRT(AVERAGE(L2:L5^2))</f>
         <v>7.0751325075930557E-2</v>
       </c>
-      <c r="N2" s="19">
+      <c r="N2" s="47">
         <f>M2/(G2*I2)*1000*100</f>
         <v>10.990228018334049</v>
       </c>
@@ -15157,7 +15180,7 @@
         <f t="array" ref="M8">SQRT(AVERAGE(L8:L11^2))</f>
         <v>7.1251315777324423E-2</v>
       </c>
-      <c r="N8" s="19">
+      <c r="N8" s="47">
         <f>M8/(G8*I8)*1000*100</f>
         <v>11.160408293313711</v>
       </c>
@@ -15367,7 +15390,7 @@
         <f t="array" ref="M14">SQRT(AVERAGE(L14:L17^2))</f>
         <v>7.0751325075930557E-2</v>
       </c>
-      <c r="N14" s="19">
+      <c r="N14" s="47">
         <f>M14/(G14*I14)*1000*100</f>
         <v>11.233692436139808</v>
       </c>
@@ -15577,7 +15600,7 @@
         <f t="array" ref="M20">SQRT(AVERAGE(L20:L23^2))</f>
         <v>7.3751271175485508E-2</v>
       </c>
-      <c r="N20" s="19">
+      <c r="N20" s="47">
         <f>M20/(G20*I20)*1000*100</f>
         <v>11.238776373222075</v>
       </c>
@@ -15787,7 +15810,7 @@
         <f t="array" ref="M26">SQRT(AVERAGE(L26:L29^2))</f>
         <v>6.8000000000000005E-2</v>
       </c>
-      <c r="N26" s="19">
+      <c r="N26" s="47">
         <f>M26/(G26*I26)*1000*100</f>
         <v>11.001092603959908</v>
       </c>
@@ -28912,8 +28935,8 @@
   </sheetPr>
   <dimension ref="A1:AE1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="186" workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="N41" sqref="N41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -29040,7 +29063,7 @@
         <f t="array" ref="M2">SQRT(AVERAGE(L2:L5^2))</f>
         <v>0.127</v>
       </c>
-      <c r="N2" s="19">
+      <c r="N2" s="46">
         <f>M2/(G2*I2)*1000*100</f>
         <v>20.060501798111634</v>
       </c>
@@ -29272,7 +29295,7 @@
         <f t="array" ref="M8">SQRT(AVERAGE(L8:L11^2))</f>
         <v>0.128</v>
       </c>
-      <c r="N8" s="19">
+      <c r="N8" s="47">
         <f>M8/(G8*I8)*1000*100</f>
         <v>20.160703847881287</v>
       </c>
@@ -29488,7 +29511,7 @@
         <f t="array" ref="M14">SQRT(AVERAGE(L14:L17^2))</f>
         <v>0.127</v>
       </c>
-      <c r="N14" s="19">
+      <c r="N14" s="47">
         <f>M14/(G14*I14)*1000*100</f>
         <v>20.187171711981119</v>
       </c>
@@ -29698,7 +29721,7 @@
         <f t="array" ref="M20">SQRT(AVERAGE(L20:L23^2))</f>
         <v>0.128</v>
       </c>
-      <c r="N20" s="19">
+      <c r="N20" s="47">
         <f>M20/(G20*I20)*1000*100</f>
         <v>20.100385688415383</v>
       </c>
@@ -29908,7 +29931,7 @@
         <f t="array" ref="M26">SQRT(AVERAGE(L26:L29^2))</f>
         <v>0.12950096524736796</v>
       </c>
-      <c r="N26" s="19">
+      <c r="N26" s="47">
         <f>M26/(G26*I26)*1000*100</f>
         <v>20.107660132804963</v>
       </c>
@@ -43033,7 +43056,7 @@
   </sheetPr>
   <dimension ref="A1:AE1000"/>
   <sheetViews>
-    <sheetView zoomScale="167" workbookViewId="0">
+    <sheetView zoomScale="83" workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
got the weighted avrg bc code to work
</commit_message>
<xml_diff>
--- a/50MeV_stack_analysis/50MeV_Ti_Fe_Zr_Foils.xlsx
+++ b/50MeV_stack_analysis/50MeV_Ti_Fe_Zr_Foils.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d50fdffd1f97c7a6/Dokumenter/Master/Master-project-code/50MeV_stack_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="285" documentId="14_{7FE2433E-3551-A74B-8720-1D259C5F8435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E358062F-7E5B-5E4D-AE81-C7ABE919A646}"/>
+  <xr:revisionPtr revIDLastSave="286" documentId="14_{7FE2433E-3551-A74B-8720-1D259C5F8435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{32CF8F9C-4EB5-BE41-AC7F-FC1E871FFA41}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="500" windowWidth="20320" windowHeight="14420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zr" sheetId="1" r:id="rId1"/>
@@ -710,7 +710,7 @@
   </sheetPr>
   <dimension ref="A1:AE1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
@@ -14823,7 +14823,7 @@
   </sheetPr>
   <dimension ref="A1:AE1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
       <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
@@ -28935,7 +28935,7 @@
   </sheetPr>
   <dimension ref="A1:AE1000"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="L1" workbookViewId="0">
       <selection activeCell="N41" sqref="N41"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
First commit in a long time
</commit_message>
<xml_diff>
--- a/50MeV_stack_analysis/50MeV_Ti_Fe_Zr_Foils.xlsx
+++ b/50MeV_stack_analysis/50MeV_Ti_Fe_Zr_Foils.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d50fdffd1f97c7a6/Dokumenter/Master/Master-project-code/50MeV_stack_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="286" documentId="14_{7FE2433E-3551-A74B-8720-1D259C5F8435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{32CF8F9C-4EB5-BE41-AC7F-FC1E871FFA41}"/>
+  <xr:revisionPtr revIDLastSave="368" documentId="14_{7FE2433E-3551-A74B-8720-1D259C5F8435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E56967A-563B-584E-986E-F661C3D6FBFE}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="500" windowWidth="20320" windowHeight="14420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35720" yWindow="8600" windowWidth="29960" windowHeight="19120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zr" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="33">
   <si>
     <t>Shot</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>E9</t>
+  </si>
+  <si>
+    <t>pm</t>
   </si>
 </sst>
 </file>
@@ -280,7 +283,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -387,6 +390,9 @@
     <xf numFmtId="164" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,9 +415,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -449,7 +455,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -555,7 +561,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -697,7 +703,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -710,8 +716,8 @@
   </sheetPr>
   <dimension ref="A1:AE1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+    <sheetView topLeftCell="A24" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -873,19 +879,27 @@
       <c r="F3" s="15">
         <v>24.8</v>
       </c>
-      <c r="G3" s="16"/>
+      <c r="G3" s="48" t="s">
+        <v>32</v>
+      </c>
       <c r="H3" s="16">
         <v>24.76</v>
       </c>
-      <c r="I3" s="16"/>
+      <c r="I3" s="48" t="s">
+        <v>32</v>
+      </c>
       <c r="J3" s="17">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="K3" s="18"/>
+      <c r="K3" s="43" t="s">
+        <v>32</v>
+      </c>
       <c r="L3" s="18">
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="M3" s="24"/>
+      <c r="M3" s="24" t="s">
+        <v>32</v>
+      </c>
       <c r="N3" s="19" t="s">
         <v>17</v>
       </c>
@@ -917,19 +931,29 @@
       <c r="F4" s="15">
         <v>24.84</v>
       </c>
-      <c r="G4" s="16"/>
+      <c r="G4" s="16">
+        <f>STDEV(F2:F5)</f>
+        <v>3.4034296427770241E-2</v>
+      </c>
       <c r="H4" s="16">
         <v>24.85</v>
       </c>
-      <c r="I4" s="16"/>
+      <c r="I4" s="16">
+        <f>STDEV(H2:H5)</f>
+        <v>0.25850531909421148</v>
+      </c>
       <c r="J4" s="17">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="K4" s="18"/>
+      <c r="K4" s="18">
+        <v>0</v>
+      </c>
       <c r="L4" s="18">
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="M4" s="24"/>
+      <c r="M4" s="24">
+        <v>0</v>
+      </c>
       <c r="N4" s="19"/>
       <c r="O4" s="25"/>
       <c r="P4" s="25"/>
@@ -1136,19 +1160,29 @@
       <c r="F10" s="15">
         <v>25.2</v>
       </c>
-      <c r="G10" s="16"/>
+      <c r="G10" s="16">
+        <f>STDEV(F8:F11)</f>
+        <v>4.9999999999990052E-3</v>
+      </c>
       <c r="H10" s="16">
         <v>24.78</v>
       </c>
-      <c r="I10" s="16"/>
+      <c r="I10" s="16">
+        <f>STDEV(H8:H11)</f>
+        <v>2.708012801545219E-2</v>
+      </c>
       <c r="J10" s="17">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="K10" s="18"/>
+      <c r="K10" s="18">
+        <v>0</v>
+      </c>
       <c r="L10" s="18">
         <v>0.1</v>
       </c>
-      <c r="M10" s="24"/>
+      <c r="M10" s="24">
+        <v>0</v>
+      </c>
       <c r="N10" s="19"/>
       <c r="O10" s="25"/>
       <c r="P10" s="25"/>
@@ -1346,19 +1380,29 @@
       <c r="F16" s="15">
         <v>24.75</v>
       </c>
-      <c r="G16" s="16"/>
+      <c r="G16" s="16">
+        <f>STDEV(F14:F17)</f>
+        <v>3.9157800414902508E-2</v>
+      </c>
       <c r="H16" s="16">
         <v>25.36</v>
       </c>
-      <c r="I16" s="16"/>
+      <c r="I16" s="16">
+        <f>STDEV(H14:H17)</f>
+        <v>1.5000000000000371E-2</v>
+      </c>
       <c r="J16" s="17">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="K16" s="18"/>
+      <c r="K16" s="18">
+        <v>0</v>
+      </c>
       <c r="L16" s="18">
         <v>0.10199999999999999</v>
       </c>
-      <c r="M16" s="24"/>
+      <c r="M16" s="24">
+        <v>0</v>
+      </c>
       <c r="N16" s="19"/>
       <c r="O16" s="25"/>
       <c r="P16" s="25"/>
@@ -1556,19 +1600,29 @@
       <c r="F22" s="15">
         <v>24.77</v>
       </c>
-      <c r="G22" s="16"/>
+      <c r="G22" s="16">
+        <f>STDEV(F20:F23)</f>
+        <v>3.5939764421412564E-2</v>
+      </c>
       <c r="H22" s="16">
         <v>25.43</v>
       </c>
-      <c r="I22" s="16"/>
+      <c r="I22" s="16">
+        <f>STDEV(H20:H23)</f>
+        <v>0.10144785195688881</v>
+      </c>
       <c r="J22" s="17">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="K22" s="18"/>
+      <c r="K22" s="18">
+        <v>0</v>
+      </c>
       <c r="L22" s="18">
         <v>0.10199999999999999</v>
       </c>
-      <c r="M22" s="24"/>
+      <c r="M22" s="24">
+        <v>0</v>
+      </c>
       <c r="N22" s="19"/>
       <c r="O22" s="25"/>
       <c r="P22" s="25"/>
@@ -1766,19 +1820,29 @@
       <c r="F28" s="15">
         <v>24.9</v>
       </c>
-      <c r="G28" s="16"/>
+      <c r="G28" s="16">
+        <f>STDEV(F26:F29)</f>
+        <v>3.3166247903554186E-2</v>
+      </c>
       <c r="H28" s="16">
         <v>25.53</v>
       </c>
-      <c r="I28" s="16"/>
+      <c r="I28" s="16">
+        <f>STDEV(H26:H29)</f>
+        <v>1.499999999999899E-2</v>
+      </c>
       <c r="J28" s="17">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="K28" s="18"/>
+      <c r="K28" s="18">
+        <v>0</v>
+      </c>
       <c r="L28" s="18">
         <v>0.10299999999999999</v>
       </c>
-      <c r="M28" s="24"/>
+      <c r="M28" s="24">
+        <v>0</v>
+      </c>
       <c r="N28" s="19"/>
       <c r="O28" s="25"/>
       <c r="P28" s="25"/>
@@ -14823,8 +14887,8 @@
   </sheetPr>
   <dimension ref="A1:AE1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -14986,19 +15050,27 @@
       <c r="F3" s="15">
         <v>25.3</v>
       </c>
-      <c r="G3" s="16"/>
+      <c r="G3" s="48" t="s">
+        <v>32</v>
+      </c>
       <c r="H3" s="16">
         <v>25.42</v>
       </c>
-      <c r="I3" s="16"/>
+      <c r="I3" s="48" t="s">
+        <v>32</v>
+      </c>
       <c r="J3" s="17">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="K3" s="18"/>
+      <c r="K3" s="43" t="s">
+        <v>32</v>
+      </c>
       <c r="L3" s="18">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="M3" s="24"/>
+      <c r="M3" s="24" t="s">
+        <v>32</v>
+      </c>
       <c r="N3" s="19" t="s">
         <v>17</v>
       </c>
@@ -15030,19 +15102,31 @@
       <c r="F4" s="15">
         <v>25.38</v>
       </c>
-      <c r="G4" s="16"/>
+      <c r="G4" s="16">
+        <f>STDEV(F2:F5)</f>
+        <v>4.434711565216596E-2</v>
+      </c>
       <c r="H4" s="16">
         <v>25.31</v>
       </c>
-      <c r="I4" s="16"/>
+      <c r="I4" s="16">
+        <f>STDEV(H2:H5)</f>
+        <v>6.4807406984079594E-2</v>
+      </c>
       <c r="J4" s="17">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="K4" s="18"/>
+      <c r="K4" s="18">
+        <f>STDEV(J2:J5)</f>
+        <v>0</v>
+      </c>
       <c r="L4" s="18">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="M4" s="24"/>
+      <c r="M4" s="24">
+        <f>STDEV(L2:L5)</f>
+        <v>4.9999999999999351E-4</v>
+      </c>
       <c r="N4" s="19"/>
       <c r="O4" s="25"/>
       <c r="P4" s="25"/>
@@ -15248,19 +15332,31 @@
       <c r="F10" s="15">
         <v>25.18</v>
       </c>
-      <c r="G10" s="16"/>
+      <c r="G10" s="16">
+        <f>STDEV(F8:F11)</f>
+        <v>0.14271183085738445</v>
+      </c>
       <c r="H10" s="16">
         <v>25.38</v>
       </c>
-      <c r="I10" s="16"/>
+      <c r="I10" s="16">
+        <f>STDEV(H8:H11)</f>
+        <v>6.1644140029689806E-2</v>
+      </c>
       <c r="J10" s="17">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="K10" s="18"/>
+      <c r="K10" s="18">
+        <f>STDEV(J8:J11)</f>
+        <v>0</v>
+      </c>
       <c r="L10" s="18">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="M10" s="24"/>
+      <c r="M10" s="24">
+        <f>STDEV(L8:L11)</f>
+        <v>5.0000000000000044E-4</v>
+      </c>
       <c r="N10" s="19"/>
       <c r="O10" s="25"/>
       <c r="P10" s="25"/>
@@ -15458,19 +15554,31 @@
       <c r="F16" s="15">
         <v>25.02</v>
       </c>
-      <c r="G16" s="16"/>
+      <c r="G16" s="16">
+        <f>STDEV(F14:F17)</f>
+        <v>2.3804761428476654E-2</v>
+      </c>
       <c r="H16" s="16">
         <v>25.22</v>
       </c>
-      <c r="I16" s="16"/>
+      <c r="I16" s="16">
+        <f>STDEV(H14:H17)</f>
+        <v>7.1355915428692726E-2</v>
+      </c>
       <c r="J16" s="17">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="K16" s="18"/>
+      <c r="K16" s="18">
+        <f>STDEV(J14:J17)</f>
+        <v>4.9999999999999871E-4</v>
+      </c>
       <c r="L16" s="18">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="M16" s="24"/>
+      <c r="M16" s="24">
+        <f>STDEV(L14:L17)</f>
+        <v>4.9999999999999351E-4</v>
+      </c>
       <c r="N16" s="19"/>
       <c r="O16" s="25"/>
       <c r="P16" s="25"/>
@@ -15668,19 +15776,30 @@
       <c r="F22" s="15">
         <v>25.7</v>
       </c>
-      <c r="G22" s="16"/>
+      <c r="G22" s="16">
+        <f>STDEV(F20:F23)</f>
+        <v>0.19448650338776696</v>
+      </c>
       <c r="H22" s="16">
         <v>25.82</v>
       </c>
-      <c r="I22" s="16"/>
+      <c r="I22" s="16">
+        <f>STDEV(H20:H23)</f>
+        <v>0.4821047603996465</v>
+      </c>
       <c r="J22" s="17">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="K22" s="18"/>
+      <c r="K22" s="18">
+        <v>0</v>
+      </c>
       <c r="L22" s="18">
         <v>7.2999999999999995E-2</v>
       </c>
-      <c r="M22" s="24"/>
+      <c r="M22" s="24">
+        <f>STDEV(L20:L23)</f>
+        <v>5.0000000000000044E-4</v>
+      </c>
       <c r="N22" s="19"/>
       <c r="O22" s="25"/>
       <c r="P22" s="25"/>
@@ -15878,19 +15997,29 @@
       <c r="F28" s="15">
         <v>25.51</v>
       </c>
-      <c r="G28" s="16"/>
+      <c r="G28" s="16">
+        <f>STDEV(F26:F29)</f>
+        <v>2.5819888974717396E-2</v>
+      </c>
       <c r="H28" s="16">
         <v>24.25</v>
       </c>
-      <c r="I28" s="16"/>
+      <c r="I28" s="16">
+        <f>STDEV(H26:H29)</f>
+        <v>2.1602468994692956E-2</v>
+      </c>
       <c r="J28" s="17">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="K28" s="18"/>
+      <c r="K28" s="18">
+        <v>0</v>
+      </c>
       <c r="L28" s="18">
         <v>6.8000000000000005E-2</v>
       </c>
-      <c r="M28" s="24"/>
+      <c r="M28" s="24">
+        <v>0</v>
+      </c>
       <c r="N28" s="19"/>
       <c r="O28" s="25"/>
       <c r="P28" s="25"/>
@@ -28935,8 +29064,8 @@
   </sheetPr>
   <dimension ref="A1:AE1000"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="N41" sqref="N41"/>
+    <sheetView topLeftCell="A12" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -29098,19 +29227,27 @@
       <c r="F3" s="15">
         <v>25.11</v>
       </c>
-      <c r="G3" s="16"/>
+      <c r="G3" s="48" t="s">
+        <v>32</v>
+      </c>
       <c r="H3" s="16">
         <v>25.2</v>
       </c>
-      <c r="I3" s="16"/>
+      <c r="I3" s="48" t="s">
+        <v>32</v>
+      </c>
       <c r="J3" s="17">
         <v>2.7E-2</v>
       </c>
-      <c r="K3" s="18"/>
+      <c r="K3" s="43" t="s">
+        <v>32</v>
+      </c>
       <c r="L3" s="18">
         <v>0.127</v>
       </c>
-      <c r="M3" s="24"/>
+      <c r="M3" s="24" t="s">
+        <v>32</v>
+      </c>
       <c r="N3" s="19" t="s">
         <v>17</v>
       </c>
@@ -29142,19 +29279,30 @@
       <c r="F4" s="15">
         <v>25.04</v>
       </c>
-      <c r="G4" s="16"/>
+      <c r="G4" s="16">
+        <f>STDEV(F2:F5)</f>
+        <v>3.8729833462074259E-2</v>
+      </c>
       <c r="H4" s="16">
         <v>25.25</v>
       </c>
-      <c r="I4" s="16"/>
+      <c r="I4" s="16">
+        <f>STDEV(H2:H5)</f>
+        <v>2.217355782608358E-2</v>
+      </c>
       <c r="J4" s="17">
         <v>2.7E-2</v>
       </c>
-      <c r="K4" s="18"/>
+      <c r="K4" s="18">
+        <f>STDEV(J2:J5)</f>
+        <v>5.0000000000000044E-4</v>
+      </c>
       <c r="L4" s="18">
         <v>0.127</v>
       </c>
-      <c r="M4" s="24"/>
+      <c r="M4" s="24">
+        <v>0</v>
+      </c>
       <c r="N4" s="19"/>
       <c r="O4" s="25"/>
       <c r="P4" s="25"/>
@@ -29369,19 +29517,30 @@
       <c r="F10" s="15">
         <v>24.91</v>
       </c>
-      <c r="G10" s="16"/>
+      <c r="G10" s="16">
+        <f>STDEV(F8:F11)</f>
+        <v>3.5939764421412647E-2</v>
+      </c>
       <c r="H10" s="16">
         <v>25.49</v>
       </c>
-      <c r="I10" s="16"/>
+      <c r="I10" s="16">
+        <f>STDEV(H8:H11)</f>
+        <v>1.4142135623729813E-2</v>
+      </c>
       <c r="J10" s="17">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="K10" s="18"/>
+      <c r="K10" s="18">
+        <f>STDEV(J8:J11)</f>
+        <v>5.0000000000000044E-4</v>
+      </c>
       <c r="L10" s="18">
         <v>0.128</v>
       </c>
-      <c r="M10" s="24"/>
+      <c r="M10" s="24">
+        <v>0</v>
+      </c>
       <c r="N10" s="19"/>
       <c r="O10" s="25"/>
       <c r="P10" s="25"/>
@@ -29579,19 +29738,30 @@
       <c r="F16" s="15">
         <v>24.75</v>
       </c>
-      <c r="G16" s="16"/>
+      <c r="G16" s="16">
+        <f>STDEV(F14:F17)</f>
+        <v>0.13329166015421492</v>
+      </c>
       <c r="H16" s="16">
         <v>25.5</v>
       </c>
-      <c r="I16" s="16"/>
+      <c r="I16" s="16">
+        <f>STDEV(H14:H17)</f>
+        <v>3.3166247903554186E-2</v>
+      </c>
       <c r="J16" s="17">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="K16" s="18"/>
+      <c r="K16" s="18">
+        <f>STDEV(J14:J17)</f>
+        <v>8.1649658092772682E-4</v>
+      </c>
       <c r="L16" s="43">
         <v>0.127</v>
       </c>
-      <c r="M16" s="24"/>
+      <c r="M16" s="24">
+        <v>0</v>
+      </c>
       <c r="N16" s="19"/>
       <c r="O16" s="25"/>
       <c r="P16" s="25"/>
@@ -29789,19 +29959,30 @@
       <c r="F22" s="15">
         <v>25.25</v>
       </c>
-      <c r="G22" s="16"/>
+      <c r="G22" s="16">
+        <f>STDEV(F20:F23)</f>
+        <v>4.8304589153964503E-2</v>
+      </c>
       <c r="H22" s="16">
         <v>25.32</v>
       </c>
-      <c r="I22" s="16"/>
+      <c r="I22" s="16">
+        <f>STDEV(H20:H23)</f>
+        <v>4.0824829046386013E-2</v>
+      </c>
       <c r="J22" s="17">
         <v>2.7E-2</v>
       </c>
-      <c r="K22" s="18"/>
+      <c r="K22" s="18">
+        <f>STDEV(J20:J23)</f>
+        <v>5.0000000000000044E-4</v>
+      </c>
       <c r="L22" s="18">
         <v>0.128</v>
       </c>
-      <c r="M22" s="24"/>
+      <c r="M22" s="24">
+        <v>0</v>
+      </c>
       <c r="N22" s="19"/>
       <c r="O22" s="25"/>
       <c r="P22" s="25"/>
@@ -29999,19 +30180,31 @@
       <c r="F28" s="15">
         <v>25.18</v>
       </c>
-      <c r="G28" s="16"/>
+      <c r="G28" s="16">
+        <f>STDEV(F26:F29)</f>
+        <v>1.2909944487358698E-2</v>
+      </c>
       <c r="H28" s="16">
         <v>25.68</v>
       </c>
-      <c r="I28" s="16"/>
+      <c r="I28" s="16">
+        <f>STDEV(H26:H29)</f>
+        <v>8.4606934309980189E-2</v>
+      </c>
       <c r="J28" s="17">
         <v>2.7E-2</v>
       </c>
-      <c r="K28" s="18"/>
+      <c r="K28" s="18">
+        <f>STDEV(J26:J29)</f>
+        <v>5.0000000000000044E-4</v>
+      </c>
       <c r="L28" s="18">
         <v>0.13</v>
       </c>
-      <c r="M28" s="24"/>
+      <c r="M28" s="24">
+        <f>STDEV(L26:L29)</f>
+        <v>5.7735026918962634E-4</v>
+      </c>
       <c r="N28" s="19"/>
       <c r="O28" s="25"/>
       <c r="P28" s="25"/>

</xml_diff>